<commit_message>
Updated data with DX explanations
</commit_message>
<xml_diff>
--- a/data/Behavioral/description/APQ_P.xlsx
+++ b/data/Behavioral/description/APQ_P.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Healthy Brain Network\Data Sharing\Data Dictionaries\Public Data Dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/Research/Healthy Brain Network/Data Sharing/Data Dictionaries/Public Data Dictionaries/all_data_dicts_Jan_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8265" yWindow="0" windowWidth="28800" windowHeight="18420" tabRatio="500"/>
+    <workbookView xWindow="8260" yWindow="460" windowWidth="28800" windowHeight="18420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -71,12 +74,6 @@
     <t>1. You have a friendly talk with your child</t>
   </si>
   <si>
-    <t>2. Your ket your child know when he/she is doing a good job with something</t>
-  </si>
-  <si>
-    <t>3. You threaten to punish your child and then do not actuallypunish him/her</t>
-  </si>
-  <si>
     <t>4. You volunteer to help with special activities that your child is involved with (such as sports, boy/girl scouts, church youth groups)</t>
   </si>
   <si>
@@ -348,12 +345,18 @@
   </si>
   <si>
     <t xml:space="preserve">Alabama Parenting Questionnaire (APQ) Parent-Report </t>
+  </si>
+  <si>
+    <t>2. You let your child know when he/she is doing a good job with something</t>
+  </si>
+  <si>
+    <t>3. You threaten to punish your child and then do not actually punish him/her</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1115,19 +1118,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="83.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1144,710 +1149,710 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>59</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>60</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>62</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>65</v>
       </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>66</v>
       </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>67</v>
       </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>68</v>
       </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>70</v>
       </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>71</v>
       </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>73</v>
       </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>74</v>
       </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>75</v>
       </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>76</v>
       </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>77</v>
       </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>78</v>
       </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>79</v>
       </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>36</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>80</v>
       </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>83</v>
       </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>40</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>84</v>
       </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>41</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>85</v>
       </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>42</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>86</v>
       </c>
-      <c r="C31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>87</v>
       </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>44</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>88</v>
       </c>
-      <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>45</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>89</v>
       </c>
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>46</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>90</v>
       </c>
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>47</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>91</v>
       </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>48</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>92</v>
       </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>49</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>93</v>
       </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>50</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>94</v>
       </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>51</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>95</v>
       </c>
-      <c r="C40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>96</v>
       </c>
-      <c r="C41" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C42" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" t="s">
-        <v>12</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="C44" s="5" t="s">
         <v>12</v>
       </c>
@@ -1855,86 +1860,86 @@
         <v>13</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" t="s">
         <v>12</v>
@@ -1943,10 +1948,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>